<commit_message>
Update ship classification result using HOG
</commit_message>
<xml_diff>
--- a/docs/dataset.xlsx
+++ b/docs/dataset.xlsx
@@ -16,12 +16,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test</t>
   </si>
   <si>
     <t>Train</t>
+  </si>
+  <si>
+    <t>Tropical Depression</t>
+  </si>
+  <si>
+    <t>Tropical Storm</t>
+  </si>
+  <si>
+    <t>Serve Tropical Storm</t>
+  </si>
+  <si>
+    <t>Typhoon</t>
+  </si>
+  <si>
+    <t>Extra TC</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Not Correct</t>
   </si>
 </sst>
 </file>
@@ -239,25 +260,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="121909632"/>
-        <c:axId val="121911552"/>
+        <c:axId val="98858880"/>
+        <c:axId val="98860416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121909632"/>
+        <c:axId val="98858880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121911552"/>
+        <c:crossAx val="98860416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121911552"/>
+        <c:axId val="98860416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -265,7 +286,205 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121909632"/>
+        <c:crossAx val="98858880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HOG</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$22:$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Tropical Depression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tropical Storm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Serve Tropical Storm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Typhoon</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Extra TC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$22:$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Tropical Depression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tropical Storm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Serve Tropical Storm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Typhoon</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Extra TC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$24:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="38038528"/>
+        <c:axId val="38306560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38038528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38306560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38306560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38038528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -311,6 +530,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -604,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,6 +955,63 @@
       </c>
       <c r="C9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9">
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>121</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <v>42</v>
+      </c>
+      <c r="G24">
+        <v>36</v>
+      </c>
+      <c r="H24">
+        <v>57</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>